<commit_message>
Se agregan los Factores Críticos
</commit_message>
<xml_diff>
--- a/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
+++ b/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\pCloudDrive\mauricio.camara\tituloUnap.git\2018\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994A98A6-3117-4F34-B595-5815508AF334}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A59907-B17F-40F6-9390-25CEE3363376}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="1" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>4.</t>
   </si>
@@ -231,12 +232,18 @@
   <si>
     <t>13.4 Monitorear el Involucramiento de los Interesados</t>
   </si>
+  <si>
+    <t>Área de Conocimiento</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +258,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <name val="Wingdings 2"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -267,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -410,11 +424,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -443,6 +494,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -461,17 +524,44 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,8 +882,8 @@
   </sheetPr>
   <dimension ref="B1:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,21 +898,21 @@
   <sheetData>
     <row r="1" spans="2:9" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
@@ -841,10 +931,10 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -864,10 +954,10 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="6"/>
@@ -881,10 +971,10 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="6"/>
@@ -898,10 +988,10 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="6"/>
@@ -915,10 +1005,10 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="2:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="6"/>
@@ -934,10 +1024,10 @@
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6"/>
@@ -953,10 +1043,10 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="6"/>
@@ -972,10 +1062,10 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="6"/>
@@ -991,10 +1081,10 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="6"/>
@@ -1010,10 +1100,10 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:9" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -1039,4 +1129,228 @@
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup scale="77" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33F6BE1-6AB3-4B5B-9B9B-C2C62E3F3E94}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:H14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" style="1" customWidth="1"/>
+    <col min="3" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="1" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="23"/>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="27"/>
+    </row>
+    <row r="14" spans="2:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup scale="77" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Avance en el análisis de los antecedentes históricos
</commit_message>
<xml_diff>
--- a/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
+++ b/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\pCloudDrive\mauricio.camara\tituloUnap.git\2018\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A59907-B17F-40F6-9390-25CEE3363376}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ABF1A1-B61F-4B57-BC23-5E13A5FC2C36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="1" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="2" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1 (3)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>4.</t>
   </si>
@@ -238,12 +239,48 @@
   <si>
     <t>P</t>
   </si>
+  <si>
+    <t>inicialización</t>
+  </si>
+  <si>
+    <t>dirección</t>
+  </si>
+  <si>
+    <t>planificación</t>
+  </si>
+  <si>
+    <t>calidad</t>
+  </si>
+  <si>
+    <t>personas</t>
+  </si>
+  <si>
+    <t>riesgos</t>
+  </si>
+  <si>
+    <t>Inicialización</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>Riesgos</t>
+  </si>
+  <si>
+    <t>Calidad</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Planificación</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +302,28 @@
       <name val="Wingdings 2"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -465,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -506,6 +565,33 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -524,6 +610,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -533,35 +622,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,8 +962,8 @@
   </sheetPr>
   <dimension ref="B1:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,21 +978,21 @@
   <sheetData>
     <row r="1" spans="2:9" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
@@ -1138,8 +1218,8 @@
   </sheetPr>
   <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,19 +1233,19 @@
   <sheetData>
     <row r="1" spans="2:8" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="4" t="s">
         <v>38</v>
       </c>
@@ -1183,165 +1263,165 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+    <row r="4" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="C4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="26"/>
-    </row>
-    <row r="8" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="26"/>
-    </row>
-    <row r="9" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="26"/>
-    </row>
-    <row r="11" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="26"/>
-    </row>
-    <row r="13" spans="2:8" s="24" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="32" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="27"/>
+      <c r="C13" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="2:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1353,4 +1433,212 @@
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup scale="77" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC1F3F-D9CD-4109-A3EE-41AB8ACA2BA9}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:K14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" customWidth="1"/>
+    <col min="5" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="1" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="29"/>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="34"/>
+      <c r="K4" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="35"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="36"/>
+      <c r="K5" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="35"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="36"/>
+      <c r="K6" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="36"/>
+      <c r="K7" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="K8" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="36"/>
+      <c r="K9" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="36"/>
+    </row>
+    <row r="11" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="36"/>
+    </row>
+    <row r="12" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="36"/>
+    </row>
+    <row r="13" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+    </row>
+    <row r="14" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup scale="77" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega tabla con resumen de problemáticas vs las areas de conocimiento
</commit_message>
<xml_diff>
--- a/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
+++ b/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\pCloudDrive\mauricio.camara\tituloUnap.git\2018\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ABF1A1-B61F-4B57-BC23-5E13A5FC2C36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C7864-5FFA-4F7E-9478-7C0005914952}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="2" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="3" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja1 (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1 (4)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="72">
   <si>
     <t>4.</t>
   </si>
@@ -274,6 +275,9 @@
   </si>
   <si>
     <t>Planificación</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -592,6 +596,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -621,27 +646,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -978,21 +982,21 @@
   <sheetData>
     <row r="1" spans="2:9" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="27" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
@@ -1233,19 +1237,19 @@
   <sheetData>
     <row r="1" spans="2:8" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B3" s="29"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="4" t="s">
         <v>38</v>
       </c>
@@ -1442,8 +1446,8 @@
   </sheetPr>
   <dimension ref="B1:K14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,19 +1463,19 @@
   <sheetData>
     <row r="1" spans="2:11" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="2:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B3" s="29"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="4" t="s">
         <v>38</v>
       </c>
@@ -1493,17 +1497,17 @@
       <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="34"/>
+      <c r="G4" s="24"/>
       <c r="K4" s="14" t="s">
         <v>59</v>
       </c>
@@ -1512,15 +1516,15 @@
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="36"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="26"/>
       <c r="K5" s="14" t="s">
         <v>60</v>
       </c>
@@ -1529,13 +1533,13 @@
       <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="33" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="36"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="26"/>
       <c r="K6" s="14" t="s">
         <v>61</v>
       </c>
@@ -1544,11 +1548,11 @@
       <c r="B7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="36"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="26"/>
       <c r="K7" s="14" t="s">
         <v>62</v>
       </c>
@@ -1557,15 +1561,15 @@
       <c r="B8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="36"/>
+      <c r="G8" s="26"/>
       <c r="K8" s="14" t="s">
         <v>63</v>
       </c>
@@ -1574,15 +1578,15 @@
       <c r="B9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="33" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="36"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="26"/>
       <c r="K9" s="14" t="s">
         <v>64</v>
       </c>
@@ -1591,45 +1595,45 @@
       <c r="B10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="36"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="33" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="36"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="36"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="2:11" s="14" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="38"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1641,4 +1645,194 @@
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup scale="77" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88F697E-A1BC-4E19-BC73-DCE4142D1DC0}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:H14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" customWidth="1"/>
+    <col min="5" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="1" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+    </row>
+    <row r="3" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="36"/>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="23"/>
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="2:8" s="14" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+    </row>
+    <row r="14" spans="2:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup scale="77" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cierre análisis de antecedentes históricos
</commit_message>
<xml_diff>
--- a/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
+++ b/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\pCloudDrive\mauricio.camara\tituloUnap.git\2018\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C7864-5FFA-4F7E-9478-7C0005914952}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2EB59F-DC75-4963-A3D3-1064EDA1D116}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="3" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="10605" activeTab="3" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
   <si>
     <t>4.</t>
   </si>
@@ -275,9 +275,6 @@
   </si>
   <si>
     <t>Planificación</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1223,7 +1220,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1444,7 @@
   <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1652,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,15 +1702,15 @@
       <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>71</v>
+      <c r="C4" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="D4" s="23"/>
-      <c r="E4" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>71</v>
+      <c r="E4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="G4" s="24"/>
     </row>
@@ -1721,11 +1718,11 @@
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>71</v>
+      <c r="C5" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="23"/>
@@ -1736,8 +1733,8 @@
         <v>3</v>
       </c>
       <c r="C6" s="25"/>
-      <c r="D6" s="23" t="s">
-        <v>71</v>
+      <c r="D6" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="23"/>
@@ -1759,11 +1756,11 @@
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="23"/>
-      <c r="E8" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>71</v>
+      <c r="E8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="G8" s="26"/>
     </row>
@@ -1772,11 +1769,11 @@
         <v>6</v>
       </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>71</v>
+      <c r="D9" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="26"/>
@@ -1796,11 +1793,11 @@
         <v>8</v>
       </c>
       <c r="C11" s="25"/>
-      <c r="D11" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>71</v>
+      <c r="D11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="26"/>

</xml_diff>

<commit_message>
Se aplican mejoras al TTsegún las observaciones recibidas
</commit_message>
<xml_diff>
--- a/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
+++ b/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\pCloudDrive\mauricio.camara\tituloUnap.git\2018\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2EB59F-DC75-4963-A3D3-1064EDA1D116}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C92FD2-DBBD-4E2E-ABC3-C220FB9701A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="10605" activeTab="3" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="10605" activeTab="1" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja1 (3)" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja1 (4)" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja1 (5)" sheetId="5" r:id="rId2"/>
+    <sheet name="Hoja1 (2)" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja1 (3)" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja1 (4)" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="71">
   <si>
     <t>4.</t>
   </si>
@@ -341,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -521,11 +522,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -643,6 +653,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,8 +997,8 @@
   </sheetPr>
   <dimension ref="B1:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,6 +1247,324 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A97712-5FCE-4804-B06C-9C2D52673E33}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:I18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
+    <col min="4" max="8" width="19.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="1" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
+    </row>
+    <row r="3" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="2:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="2:9" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="2:9" s="47" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+    </row>
+    <row r="9" spans="2:9" s="47" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="44"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+    </row>
+    <row r="10" spans="2:9" s="40" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="2:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="2:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="2:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="2:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="2:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="2:8" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="D11:H11"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup scale="77" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33F6BE1-6AB3-4B5B-9B9B-C2C62E3F3E94}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1436,7 +1788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC1F3F-D9CD-4109-A3EE-41AB8ACA2BA9}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1644,14 +1996,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88F697E-A1BC-4E19-BC73-DCE4142D1DC0}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se aumenta el tamaño de las letras en tablas del PMBOK
</commit_message>
<xml_diff>
--- a/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
+++ b/2018/bibliografia/TablaAreasConocimientoVsGrupos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\pCloudDrive\mauricio.camara\tituloUnap.git\2018\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C92FD2-DBBD-4E2E-ABC3-C220FB9701A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08904394-A223-43B4-B8CD-2BF84490F0BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="10605" activeTab="1" xr2:uid="{287DBD36-9969-4355-B6AD-EF9F2DA74A10}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -654,28 +654,82 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1251,306 +1305,307 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I18"/>
+  <dimension ref="B1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="8" width="19.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="1" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="1.140625" style="56" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="55" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="56" customWidth="1"/>
+    <col min="4" max="8" width="21.85546875" style="56" customWidth="1"/>
+    <col min="9" max="9" width="1" style="56" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:9" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="34" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35"/>
-    </row>
-    <row r="3" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="4" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
+    </row>
+    <row r="3" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="I3" s="57"/>
+    </row>
+    <row r="4" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="50" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:9" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="49"/>
+      <c r="E5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="49"/>
+      <c r="G5" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="2:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="H5" s="50"/>
+    </row>
+    <row r="6" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="B6" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="49"/>
+      <c r="E6" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="49"/>
+      <c r="G6" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="2:9" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
+      <c r="H6" s="50"/>
+    </row>
+    <row r="7" spans="2:9" ht="132" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="2:9" s="47" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-    </row>
-    <row r="9" spans="2:9" s="47" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-    </row>
-    <row r="10" spans="2:9" s="40" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="41"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
+      <c r="H7" s="54"/>
+    </row>
+    <row r="8" spans="2:9" s="61" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+    </row>
+    <row r="9" spans="2:9" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+    </row>
+    <row r="10" spans="2:9" s="65" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="62"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="34" t="s">
+      <c r="C11" s="41"/>
+      <c r="D11" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="4" t="s">
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43"/>
+    </row>
+    <row r="12" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="2:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="I12" s="57"/>
+    </row>
+    <row r="13" spans="2:9" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="49"/>
+      <c r="E13" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="2:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="H13" s="50"/>
+    </row>
+    <row r="14" spans="2:9" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6" t="s">
+      <c r="D14" s="49"/>
+      <c r="E14" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="2:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+      <c r="H14" s="50"/>
+    </row>
+    <row r="15" spans="2:9" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="49"/>
+      <c r="E15" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="2:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="H15" s="50"/>
+    </row>
+    <row r="16" spans="2:9" ht="300" x14ac:dyDescent="0.25">
+      <c r="B16" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6" t="s">
+      <c r="D16" s="49"/>
+      <c r="E16" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="2:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="H16" s="50"/>
+    </row>
+    <row r="17" spans="2:8" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6" t="s">
+      <c r="D17" s="49"/>
+      <c r="E17" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="2:8" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
+      <c r="H17" s="50"/>
+    </row>
+    <row r="18" spans="2:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="9"/>
-    </row>
+      <c r="H18" s="54"/>
+    </row>
+    <row r="19" spans="2:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:C3"/>

</xml_diff>